<commit_message>
Debug & update:nanputo history
</commit_message>
<xml_diff>
--- a/南普陀寺歷任主持簡史表(橫式).xlsx
+++ b/南普陀寺歷任主持簡史表(橫式).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>國強長老</t>
   </si>
@@ -98,13 +98,7 @@
     <t>南普陀寺第1屆佛學院開辦</t>
   </si>
   <si>
-    <t>台中慈善寺主持交給振光長老</t>
-  </si>
-  <si>
     <t>任南普陀佛學院總務主任</t>
-  </si>
-  <si>
-    <t>因見能海長老穿慈航大師的南傳袈裟，南普陀佛學院自此改穿南傳袈裟</t>
   </si>
   <si>
     <t>任台中慈明寺佛學院訓導主任</t>
@@ -195,6 +189,18 @@
   </si>
   <si>
     <t>接南普陀寺主持。南普陀寺第3屆佛學院開辦(相續至今第13屆)。創辦第1屆台中齋僧大會(相續至今)</t>
+  </si>
+  <si>
+    <t>台中慈善寺主持交給振光長老，任南普陀佛學院教務主任</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>任南普陀佛學院教務主任</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>因見能學長老穿慈航大師的南傳袈裟，南普陀佛學院自此改穿南傳袈裟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -707,8 +713,8 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -735,7 +741,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -871,7 +877,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H10" s="3"/>
     </row>
@@ -901,7 +907,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H12" s="3"/>
     </row>
@@ -917,7 +923,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -988,7 +994,7 @@
         <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>13</v>
@@ -996,7 +1002,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1041,14 +1047,14 @@
         <v>26</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="48.6" x14ac:dyDescent="0.3">
@@ -1056,7 +1062,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1064,7 +1070,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1072,7 +1078,7 @@
         <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1086,7 +1092,7 @@
         <v>56</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1106,7 +1112,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1114,7 +1120,7 @@
         <v>61</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1128,7 +1134,7 @@
         <v>67</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1142,15 +1148,17 @@
         <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1162,7 +1170,7 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1175,7 +1183,7 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1188,15 +1196,15 @@
         <v>76</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1206,10 +1214,10 @@
         <v>77</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1224,7 +1232,7 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1238,7 +1246,7 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1251,7 +1259,7 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1265,16 +1273,16 @@
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1299,7 +1307,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>

</xml_diff>